<commit_message>
Final use case, final vas, class diagram, project explorer, scrum sheet.
Note scrum sheet incomplete because work hours not given to documenter
</commit_message>
<xml_diff>
--- a/docs/SE Project - Agile and Scrum Sheets.xlsx
+++ b/docs/SE Project - Agile and Scrum Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mnscu-my.sharepoint.com/personal/py8380gj_go_minnstate_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BC0F09-BEC1-4831-B8B1-A18B3CCCF5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBB3A1C4-FC3F-4C3D-B40C-F2552F1D8364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Composition" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="255">
   <si>
     <t>Team Name:</t>
   </si>
@@ -326,6 +326,72 @@
     <t>Ex: Completed, Assigned (Spring #), Backlog</t>
   </si>
   <si>
+    <t>Post-order customer wants to track delivery</t>
+  </si>
+  <si>
+    <t>Team brainstorm</t>
+  </si>
+  <si>
+    <t>CartUI, DB</t>
+  </si>
+  <si>
+    <t>2 hrs.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Unassigned</t>
+  </si>
+  <si>
+    <t>Password Management</t>
+  </si>
+  <si>
+    <t>Customers want to login using the API of another service they use (login with Meta, Apple, etc.)</t>
+  </si>
+  <si>
+    <t>LoginUI, DBObject</t>
+  </si>
+  <si>
+    <t>&lt;1 hr.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Customers want to login using FaceID</t>
+  </si>
+  <si>
+    <t>LoginUI, DBObject, Controllers</t>
+  </si>
+  <si>
+    <t>6 hrs.</t>
+  </si>
+  <si>
+    <t>Staff wants a revamp of menu customization</t>
+  </si>
+  <si>
+    <t>Employee UIs (manager role), DBObject</t>
+  </si>
+  <si>
+    <t>5 hrs.</t>
+  </si>
+  <si>
+    <t>Customers would like to use Apple pay and other convenient payment services to order food</t>
+  </si>
+  <si>
+    <t>CartUI, DB, controllers</t>
+  </si>
+  <si>
+    <t>Managers should be able to remove former employees from the system</t>
+  </si>
+  <si>
+    <t>A new ManagerUI</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
     <t>Understanding the Problem</t>
   </si>
   <si>
@@ -341,7 +407,112 @@
     <t>Brief description of output</t>
   </si>
   <si>
-    <t xml:space="preserve">Understanding the problem </t>
+    <t>Vision and Scope</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>Start to vision and scope</t>
+  </si>
+  <si>
+    <t>Finishing vision and scope</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>A concensus on what to focus on</t>
+  </si>
+  <si>
+    <t>Use Case Tables</t>
+  </si>
+  <si>
+    <t>UC diagram on board, UC tables</t>
+  </si>
+  <si>
+    <t>Login Components</t>
+  </si>
+  <si>
+    <t>Understanding of how to make login process function</t>
+  </si>
+  <si>
+    <t>Login Function</t>
+  </si>
+  <si>
+    <t>Finishing login, dummy credentials and items</t>
+  </si>
+  <si>
+    <t>Employee table and menu</t>
+  </si>
+  <si>
+    <t>New employee table, menu</t>
+  </si>
+  <si>
+    <t>GitHub Repo</t>
+  </si>
+  <si>
+    <t>Team Meeting/ Dawson and Nicholas</t>
+  </si>
+  <si>
+    <t>Codebase genesis, creating branches, verifying git works on machines, merging code</t>
+  </si>
+  <si>
+    <t>Trying to figure out what to accomplish in Sprint 2</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Refining goals for sprint 2</t>
+  </si>
+  <si>
+    <t>Ordering our priorities for Sprint 2</t>
+  </si>
+  <si>
+    <t>A list of Use Cases + Features that the team determined would be of the highest priority and value to the user</t>
+  </si>
+  <si>
+    <t>Discussing a proper customer UI</t>
+  </si>
+  <si>
+    <t>Rough blueprint for customer UI, delegated to team member martin</t>
+  </si>
+  <si>
+    <t>Discussing backend controllers rework</t>
+  </si>
+  <si>
+    <t>Properly diagrammed models of the control structure behind the project</t>
+  </si>
+  <si>
+    <t>Discussing session logging process (employee timeout)</t>
+  </si>
+  <si>
+    <t>Cohesive idea about how session logging should work</t>
+  </si>
+  <si>
+    <t>Finalizing customer page layout</t>
+  </si>
+  <si>
+    <t>A clear, concise customer page layout and refining website goals</t>
+  </si>
+  <si>
+    <t>Finishing cart system analysis</t>
+  </si>
+  <si>
+    <t>Finalizing cart, ordering process in the system</t>
+  </si>
+  <si>
+    <t>Evaluating Project Progress</t>
+  </si>
+  <si>
+    <t>Common understanding of where the project stands</t>
+  </si>
+  <si>
+    <t>Merging final code together and testing for presentation</t>
+  </si>
+  <si>
+    <t>Merged final code together, final tests complete</t>
   </si>
   <si>
     <t>General Description of Components</t>
@@ -356,23 +527,293 @@
     <t>Team Members responsible</t>
   </si>
   <si>
+    <t>landing page</t>
+  </si>
+  <si>
+    <t>Landing page for user to access and use to go to login page</t>
+  </si>
+  <si>
+    <t>Kevin Robles</t>
+  </si>
+  <si>
+    <t>Login page</t>
+  </si>
+  <si>
+    <t>Page to login and register</t>
+  </si>
+  <si>
+    <t>Kevin, Martin, Sheikh</t>
+  </si>
+  <si>
+    <t>Menu page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page to view menu items </t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Session handling</t>
+  </si>
+  <si>
+    <t>Times out inactive users and manages logged in ones</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Database object</t>
+  </si>
+  <si>
+    <t>Handles persistent data storage</t>
+  </si>
+  <si>
+    <t>View Menu Controller</t>
+  </si>
+  <si>
+    <t>Passes menu items from back end to front end</t>
+  </si>
+  <si>
+    <t>Praise</t>
+  </si>
+  <si>
+    <t>Login/Create Account Controller</t>
+  </si>
+  <si>
+    <t>Handles login process</t>
+  </si>
+  <si>
+    <t>"Add to cart" controller</t>
+  </si>
+  <si>
+    <t>Handles cart state</t>
+  </si>
+  <si>
+    <t>Nick/Praise</t>
+  </si>
+  <si>
+    <t>Food item queue</t>
+  </si>
+  <si>
+    <t>handles food item queue</t>
+  </si>
+  <si>
+    <t>Cart page</t>
+  </si>
+  <si>
+    <t>displays the cart</t>
+  </si>
+  <si>
+    <t>Order queue page</t>
+  </si>
+  <si>
+    <t>displays the order queue</t>
+  </si>
+  <si>
+    <t>Customer Menu</t>
+  </si>
+  <si>
+    <t>Shows menu for customers</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Customer Login</t>
+  </si>
+  <si>
+    <t>Allows customers to login</t>
+  </si>
+  <si>
+    <t>Customer Landing Page</t>
+  </si>
+  <si>
+    <t>Landing page for customers</t>
+  </si>
+  <si>
+    <t>Customer Search Page</t>
+  </si>
+  <si>
+    <t>Searching functionality for customers</t>
+  </si>
+  <si>
+    <t>Customer Profile Page</t>
+  </si>
+  <si>
+    <t>Customer user profile</t>
+  </si>
+  <si>
+    <t>Customer Cart Page</t>
+  </si>
+  <si>
+    <t>Customer cart page</t>
+  </si>
+  <si>
     <t>Creating the Model/UML diagram</t>
   </si>
   <si>
+    <t>*Unless otherwise specified, all diagrammed ouputs were made on platform DRAWIO</t>
+  </si>
+  <si>
+    <t>UC Diagram</t>
+  </si>
+  <si>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>drawing on board</t>
+  </si>
+  <si>
+    <t>Sys Seq</t>
+  </si>
+  <si>
+    <t>Orig SysSeq</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Orig Classes</t>
+  </si>
+  <si>
+    <t>UC Table</t>
+  </si>
+  <si>
+    <t>74 (agg.)</t>
+  </si>
+  <si>
+    <t>Updated UC Table</t>
+  </si>
+  <si>
+    <t>Updated UC</t>
+  </si>
+  <si>
+    <t>Updated SysSeq</t>
+  </si>
+  <si>
+    <t>Updated Classes</t>
+  </si>
+  <si>
+    <t>Seq Diagram UC</t>
+  </si>
+  <si>
+    <t>Updated Seq diagram</t>
+  </si>
+  <si>
     <t>Writing code</t>
   </si>
   <si>
+    <t>No other work time given to documenter</t>
+  </si>
+  <si>
+    <t>setting up database</t>
+  </si>
+  <si>
+    <t>Nick Moen</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Because the database I already had set up for our previous project, it did not take long to get it setup for this project.</t>
+  </si>
+  <si>
+    <t>create account controller</t>
+  </si>
+  <si>
+    <t>3 hour</t>
+  </si>
+  <si>
+    <t>Sets up account creation in the database</t>
+  </si>
+  <si>
+    <t>login controller</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Validates user credintials</t>
+  </si>
+  <si>
+    <t>fetch menu from database and display on interface</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Display food menu on interface(I did not write the backend controller)</t>
+  </si>
+  <si>
+    <t>Session class on employee</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>Keep track of user sessions</t>
+  </si>
+  <si>
+    <t>create account/login controller for customers</t>
+  </si>
+  <si>
+    <t>customer create account and login</t>
+  </si>
+  <si>
+    <t>session class on customer</t>
+  </si>
+  <si>
+    <t>Keep track of user sessions for customer application</t>
+  </si>
+  <si>
+    <t>Sessions</t>
+  </si>
+  <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <t>Keeping track of user windows and using session variables</t>
+  </si>
+  <si>
+    <t>Customer order controller</t>
+  </si>
+  <si>
+    <t>20 minutes</t>
+  </si>
+  <si>
+    <t>I only programmed the remove order part and fixed some code that Praise wrote</t>
+  </si>
+  <si>
+    <t>Frontend order object</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>Made the data structure in the frontend that stores the order. Also structured the tables in javascript that display the table to user.</t>
+  </si>
+  <si>
     <t>Testing the code - # runs per session</t>
   </si>
   <si>
+    <t>Testing data not given to documenter</t>
+  </si>
+  <si>
     <t>Revisions based on Testing</t>
+  </si>
+  <si>
+    <t>Nick revised sesh 11/28/2022</t>
+  </si>
+  <si>
+    <t>I'm sure others have revised based on testing as well, but communication hasn't been clear on that</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -556,6 +997,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -738,7 +1186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1022,6 +1470,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1067,7 +1563,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1134,6 +1630,22 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1472,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1538,95 +2050,95 @@
     </row>
     <row r="8" spans="2:16" ht="15" thickBot="1"/>
     <row r="9" spans="2:16">
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
     </row>
     <row r="10" spans="2:16">
-      <c r="I10" s="35"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="37"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="I11" s="35"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="37"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43"/>
     </row>
     <row r="13" spans="2:16">
-      <c r="I13" s="35"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
     </row>
     <row r="14" spans="2:16">
-      <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
     </row>
     <row r="15" spans="2:16">
-      <c r="I15" s="35"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="43"/>
     </row>
     <row r="16" spans="2:16">
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="37"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="43"/>
     </row>
     <row r="17" spans="9:13">
-      <c r="I17" s="35"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
     </row>
     <row r="18" spans="9:13">
-      <c r="I18" s="35"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="37"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="43"/>
     </row>
     <row r="19" spans="9:13">
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="43"/>
     </row>
     <row r="20" spans="9:13">
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="37"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="43"/>
     </row>
     <row r="21" spans="9:13" ht="15" thickBot="1">
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1639,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="C3:G27"/>
+  <dimension ref="C3:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1652,110 +2164,116 @@
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="3:7">
+    <row r="3" spans="3:8">
+      <c r="C3" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" spans="3:8">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="28.9">
+    <row r="5" spans="3:8" ht="28.9">
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
+        <v>120</v>
+      </c>
+      <c r="H5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8">
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="3:7">
+      <c r="H6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8">
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:8">
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:8">
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:8">
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:8">
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:8">
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:8">
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:8">
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:8">
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:8">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1851,7 +2369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1869,14 +2387,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15">
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="3" spans="2:13">
       <c r="B3" s="2" t="s">
@@ -2068,7 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="B14" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2485,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B94F3B-134F-4B75-9DE6-79084AAF604E}">
-  <dimension ref="C4:J36"/>
+  <dimension ref="C4:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2497,14 +3015,15 @@
     <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="43.15">
+    <row r="4" spans="3:11" ht="43.15">
       <c r="C4" s="3" t="s">
         <v>78</v>
       </c>
@@ -2530,7 +3049,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="43.15">
+    <row r="5" spans="3:11" ht="43.15">
       <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
@@ -2556,67 +3075,172 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="3:10">
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="3:10">
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="3:10">
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="3:10">
+    <row r="6" spans="3:11" ht="30.75">
+      <c r="C6" s="9">
+        <f ca="1">ROUND(RAND()*100, 0)</f>
+        <v>86</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="30">
+        <v>44882</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="60.75">
+      <c r="C7" s="9">
+        <f t="shared" ref="C7:C11" ca="1" si="0">ROUND(RAND()*100, 0)</f>
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="30">
+        <v>44882</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="30.75">
+      <c r="C8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="30">
+        <v>44883</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" ht="45.75">
+      <c r="C9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="30">
+        <v>44883</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="60.75">
+      <c r="C10" s="9">
+        <f ca="1">ROUND(RAND()*100, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="30">
+        <v>44883</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="45.75">
+      <c r="C11" s="35">
+        <f ca="1">ROUND(RAND()*100, 0)</f>
+        <v>90</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="30">
+        <v>44893</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -2626,7 +3250,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="3:10">
+    <row r="13" spans="3:11">
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -2636,7 +3260,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="3:10">
+    <row r="14" spans="3:11">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -2646,7 +3270,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="3:10">
+    <row r="15" spans="3:11">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -2656,7 +3280,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:11">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -2876,13 +3500,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
@@ -2890,155 +3514,319 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
-      <c r="C2" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="4" spans="3:7" ht="28.9">
       <c r="C4" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="28.9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="30.75">
       <c r="C5" s="29">
+        <v>44838</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="6">
+        <v>63</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="30.75">
+      <c r="C6" s="29">
         <v>44840</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
+      <c r="D6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="6">
         <v>90</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="3:7">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="3:7">
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="3:7">
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="3:7">
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="3:7">
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="3:7">
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="30.75">
+      <c r="C7" s="29">
+        <v>44845</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="6">
+        <v>54</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="30.75">
+      <c r="C8" s="29">
+        <v>44847</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="6">
+        <v>77</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="60.75">
+      <c r="C9" s="29">
+        <v>44852</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="60.75">
+      <c r="C10" s="29">
+        <v>44854</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="6">
+        <v>45</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="45.75">
+      <c r="C11" s="29">
+        <v>44858</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="6">
+        <v>55</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="106.5">
+      <c r="C12" s="29">
+        <v>44859</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="6">
+        <v>94</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="60.75">
+      <c r="C13" s="29">
+        <v>44866</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="32">
+        <v>38</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="121.5">
+      <c r="C14" s="31">
+        <v>44868</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="33">
+        <v>85</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="76.5">
+      <c r="C15" s="29">
+        <v>44873</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="6">
+        <v>81</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="91.5">
+      <c r="C16" s="29">
+        <v>44875</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="6">
+        <v>73</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="76.5">
+      <c r="C17" s="29">
+        <v>44880</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="6">
+        <v>31</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="76.5">
+      <c r="C18" s="29">
+        <v>44882</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="6">
+        <v>65</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="45.75">
+      <c r="C19" s="29">
+        <v>44891</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="6">
+        <v>71</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="60.75">
+      <c r="C20" s="29">
+        <v>44893</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="6">
+        <v>117</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="60.75">
+      <c r="C21" s="29">
+        <v>44894</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="6">
+        <v>92</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" s="5"/>
@@ -3085,10 +3873,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B3:D22"/>
+  <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3100,99 +3888,206 @@
   <sheetData>
     <row r="3" spans="2:4" ht="28.9">
       <c r="C3" s="25" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="28.9">
       <c r="B6" s="9" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="45.75">
+      <c r="B7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15">
+      <c r="B8" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15">
+      <c r="B9" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30.75">
+      <c r="B10" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30.75">
+      <c r="B11" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30.75">
+      <c r="B12" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="30.75">
+      <c r="B13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30.75">
+      <c r="B14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15">
+      <c r="B15" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15">
+      <c r="B16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15">
+      <c r="B17" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15">
+      <c r="B18" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15">
+      <c r="B19" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30.75">
+      <c r="B20" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="30.75">
+      <c r="B21" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30.75">
+      <c r="B22" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15">
+      <c r="B23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3202,10 +4097,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="C2:G26"/>
+  <dimension ref="C2:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3215,117 +4110,200 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
-      <c r="C2" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-    </row>
-    <row r="3" spans="3:7">
+    <row r="2" spans="3:8">
+      <c r="C2" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+    </row>
+    <row r="3" spans="3:8">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:7" ht="28.9">
+    <row r="4" spans="3:8" ht="28.9">
       <c r="C4" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7">
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="3:7">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="3:7">
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="3:7">
+        <v>120</v>
+      </c>
+      <c r="H4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="30.75">
+      <c r="C5" s="29">
+        <v>44847</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="6">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="15">
+      <c r="C6" s="29">
+        <v>44847</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="6">
+        <v>43</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="30.75">
+      <c r="C7" s="29">
+        <v>44848</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="6">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="30.75">
+      <c r="C8" s="29">
+        <v>44847</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="15">
+      <c r="C9" s="29">
+        <v>44876</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="6">
+        <v>55</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="15">
+      <c r="C10" s="29">
+        <v>44885</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" s="6">
+        <v>89</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="30.75">
+      <c r="C11" s="29">
+        <v>44885</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="6">
+        <v>47</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="30.75">
+      <c r="C12" s="29">
+        <v>44894</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F12" s="6">
+        <v>53</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:8">
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:8">
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:8">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -3412,10 +4390,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="C3:G27"/>
+  <dimension ref="C3:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3425,110 +4403,213 @@
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="3:7">
+    <row r="3" spans="3:8">
+      <c r="C3" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" spans="3:8">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="28.9">
+    <row r="5" spans="3:8" ht="28.9">
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="3:7">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="3:7">
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="3:7">
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="3:7">
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="3:7">
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="3:7">
+        <v>120</v>
+      </c>
+      <c r="H5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="106.5">
+      <c r="C6" s="29">
+        <v>44844</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="45.75">
+      <c r="C7" s="29">
+        <v>44849</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="30.75">
+      <c r="C8" s="29">
+        <v>44849</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="60.75">
+      <c r="C9" s="29">
+        <v>44850</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="30.75">
+      <c r="C10" s="29">
+        <v>44877</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="45.75">
+      <c r="C11" s="29">
+        <v>44883</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="60.75">
+      <c r="C12" s="29">
+        <v>44883</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="60.75">
+      <c r="C13" s="29">
+        <v>44893</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="76.5">
+      <c r="C14" s="29">
+        <v>44894</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="121.5">
+      <c r="C15" s="29">
+        <v>44894</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -3611,6 +4692,27 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3622,10 +4724,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="C3:G27"/>
+  <dimension ref="C3:H27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3637,110 +4739,113 @@
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="3:7">
+    <row r="3" spans="3:8">
+      <c r="C3" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" spans="3:8">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="28.9">
+    <row r="5" spans="3:8" ht="28.9">
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
+        <v>120</v>
+      </c>
+      <c r="H5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8">
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:8">
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:8">
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:8">
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:8">
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:8">
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:8">
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:8">
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:8">
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:8">
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:8">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>

</xml_diff>